<commit_message>
Improve code generation templates
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08A9AB82-2AF3-4655-AE78-B333BF28148B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F036A9-152B-4C7D-BC94-1A468711A84D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="76">
   <si>
     <t>ratio</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Hz</t>
   </si>
   <si>
-    <t>enum:4</t>
-  </si>
-  <si>
     <t>modDepth</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>makeUpGain</t>
   </si>
   <si>
-    <t>Ring Modulator</t>
-  </si>
-  <si>
     <t>Carrier Frequency</t>
   </si>
   <si>
@@ -192,7 +186,79 @@
     <t>Carrier Freq</t>
   </si>
   <si>
-    <t>enum:5</t>
+    <t>enum count</t>
+  </si>
+  <si>
+    <t>Distortion</t>
+  </si>
+  <si>
+    <t>Distortion Type</t>
+  </si>
+  <si>
+    <t>distType</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>ParametricEQ</t>
+  </si>
+  <si>
+    <t>Centre Frequency</t>
+  </si>
+  <si>
+    <t>centreFreq</t>
+  </si>
+  <si>
+    <t>Centre Freq</t>
+  </si>
+  <si>
+    <t>centreFreqHz</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>filterQ</t>
+  </si>
+  <si>
+    <t>WahWah</t>
+  </si>
+  <si>
+    <t>AutoWah</t>
+  </si>
+  <si>
+    <t>LFO Width</t>
+  </si>
+  <si>
+    <t>sec</t>
+  </si>
+  <si>
+    <t>attackTimeSec</t>
+  </si>
+  <si>
+    <t>Decay Time</t>
+  </si>
+  <si>
+    <t>decay</t>
+  </si>
+  <si>
+    <t>decayTimeSec</t>
+  </si>
+  <si>
+    <t>Envelope Width</t>
+  </si>
+  <si>
+    <t>envWidth</t>
+  </si>
+  <si>
+    <t>Env Width</t>
+  </si>
+  <si>
+    <t>envWidthHz</t>
+  </si>
+  <si>
+    <t>RingMod</t>
   </si>
 </sst>
 </file>
@@ -591,22 +657,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="2" customWidth="1"/>
+    <col min="6" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -620,25 +686,28 @@
         <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -651,31 +720,23 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>-100</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>12</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -688,18 +749,17 @@
       <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" t="s">
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="K4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
@@ -709,86 +769,81 @@
       <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>0.1</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>10</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="I5" s="2"/>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B6" t="s">
         <v>32</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>100</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>50</v>
       </c>
-      <c r="I6" s="2"/>
-      <c r="J6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
@@ -798,18 +853,17 @@
       <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" t="s">
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
@@ -819,43 +873,46 @@
       <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>10</v>
       </c>
-      <c r="J10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>100</v>
+      </c>
+      <c r="K11" t="s">
         <v>47</v>
       </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>100</v>
-      </c>
-      <c r="J11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -868,22 +925,23 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>20</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>1</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -893,26 +951,29 @@
       <c r="D14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>0.1</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>80</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>15</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>0.1</v>
       </c>
-      <c r="J14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -922,26 +983,29 @@
       <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>0.1</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>1000</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>100</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>0.1</v>
       </c>
-      <c r="J15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
@@ -951,26 +1015,29 @@
       <c r="D16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>-60</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
       </c>
       <c r="H16" s="2">
         <v>0</v>
       </c>
       <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
         <v>0.5</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -980,31 +1047,427 @@
       <c r="D17" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>0</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>24</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>0</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>0.1</v>
       </c>
-      <c r="J17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="K19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-24</v>
+      </c>
+      <c r="H20" s="2">
+        <v>24</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G22" s="2">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2">
+        <v>20000</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>20</v>
+      </c>
+      <c r="I23" s="2">
+        <v>2</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="2">
+        <v>-12</v>
+      </c>
+      <c r="H24" s="2">
+        <v>12</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="2">
+        <v>400</v>
+      </c>
+      <c r="H26" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I26" s="2">
+        <v>400</v>
+      </c>
+      <c r="K26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <v>20</v>
+      </c>
+      <c r="I27" s="2">
+        <v>5</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="2">
+        <v>200</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I29" s="2">
+        <v>350</v>
+      </c>
+      <c r="K29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="2">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2">
+        <v>20</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H31" s="2">
+        <v>20</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2</v>
+      </c>
+      <c r="K31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="I33" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>2</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="K34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>4000</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new Delay effect
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386A04E7-60A8-4C9A-886A-615FE2926263}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC82081F-D986-424A-A0A8-48980966138B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="102">
   <si>
     <t>ratio</t>
   </si>
@@ -310,6 +310,33 @@
   </si>
   <si>
     <t>numFilters</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Delay Time</t>
+  </si>
+  <si>
+    <t>delayTime</t>
+  </si>
+  <si>
+    <t>delaySec</t>
+  </si>
+  <si>
+    <t>Dry Mix Level</t>
+  </si>
+  <si>
+    <t>dryLevel</t>
+  </si>
+  <si>
+    <t>Wet Mix Level</t>
+  </si>
+  <si>
+    <t>wetLevel</t>
+  </si>
+  <si>
+    <t>Delay Mix Level</t>
   </si>
 </sst>
 </file>
@@ -708,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I43" sqref="I43"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,6 +1784,134 @@
         <v>92</v>
       </c>
     </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" t="s">
+        <v>94</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H46" s="2">
+        <v>2</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2">
+        <v>99.5</v>
+      </c>
+      <c r="I47" s="2">
+        <v>75</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
+        <v>98</v>
+      </c>
+      <c r="D48" t="s">
+        <v>97</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>100</v>
+      </c>
+      <c r="I48" s="2">
+        <v>100</v>
+      </c>
+      <c r="J48" s="2">
+        <v>1</v>
+      </c>
+      <c r="K48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" t="s">
+        <v>101</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G49" s="2">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>100</v>
+      </c>
+      <c r="I49" s="2">
+        <v>50</v>
+      </c>
+      <c r="J49" s="2">
+        <v>1</v>
+      </c>
+      <c r="K49" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new Ping-Pong Delay effect
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC82081F-D986-424A-A0A8-48980966138B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6024800-EC8E-47DB-B8E7-24D90F04F9B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="111">
   <si>
     <t>ratio</t>
   </si>
@@ -337,6 +337,33 @@
   </si>
   <si>
     <t>Delay Mix Level</t>
+  </si>
+  <si>
+    <t>PingPongDelay</t>
+  </si>
+  <si>
+    <t>L-R Delay Time</t>
+  </si>
+  <si>
+    <t>Left Delay Time</t>
+  </si>
+  <si>
+    <t>delayTimeL</t>
+  </si>
+  <si>
+    <t>delaySecL</t>
+  </si>
+  <si>
+    <t>Right Delay Time</t>
+  </si>
+  <si>
+    <t>delayTimeR</t>
+  </si>
+  <si>
+    <t>R-L Delay Time</t>
+  </si>
+  <si>
+    <t>delaySecR</t>
   </si>
 </sst>
 </file>
@@ -735,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1912,6 +1939,134 @@
         <v>100</v>
       </c>
     </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" t="s">
+        <v>103</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G51" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H51" s="2">
+        <v>2</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J51" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K51" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H52" s="2">
+        <v>2</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" t="s">
+        <v>86</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" s="2">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2">
+        <v>99.5</v>
+      </c>
+      <c r="I53" s="2">
+        <v>75</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" t="s">
+        <v>101</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G54" s="2">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2">
+        <v>100</v>
+      </c>
+      <c r="I54" s="2">
+        <v>50</v>
+      </c>
+      <c r="J54" s="2">
+        <v>1</v>
+      </c>
+      <c r="K54" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new Vibrato effect
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6024800-EC8E-47DB-B8E7-24D90F04F9B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20CFC2E-6915-4514-AF61-CDF047296A40}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="115">
   <si>
     <t>ratio</t>
   </si>
@@ -364,6 +364,18 @@
   </si>
   <si>
     <t>delaySecR</t>
+  </si>
+  <si>
+    <t>Vibrato</t>
+  </si>
+  <si>
+    <t>Interpolation Type</t>
+  </si>
+  <si>
+    <t>interpType</t>
+  </si>
+  <si>
+    <t>interpolationType</t>
   </si>
 </sst>
 </file>
@@ -762,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,6 +2079,116 @@
         <v>100</v>
       </c>
     </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" t="s">
+        <v>29</v>
+      </c>
+      <c r="D56" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" s="2">
+        <v>4</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0</v>
+      </c>
+      <c r="K56" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H57" s="2">
+        <v>5</v>
+      </c>
+      <c r="I57" s="2">
+        <v>2</v>
+      </c>
+      <c r="J57" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B58" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="J58" s="2">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K58" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" t="s">
+        <v>112</v>
+      </c>
+      <c r="E59" s="2">
+        <v>3</v>
+      </c>
+      <c r="I59" s="2">
+        <v>1</v>
+      </c>
+      <c r="K59" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new Flanger effect
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20CFC2E-6915-4514-AF61-CDF047296A40}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1E391C-7C4A-4F25-84B8-1A00EB08D375}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="120">
   <si>
     <t>ratio</t>
   </si>
@@ -376,6 +376,21 @@
   </si>
   <si>
     <t>interpolationType</t>
+  </si>
+  <si>
+    <t>Flanger</t>
+  </si>
+  <si>
+    <t>Min Delay</t>
+  </si>
+  <si>
+    <t>minDelay</t>
+  </si>
+  <si>
+    <t>minDelayMs</t>
+  </si>
+  <si>
+    <t>sweepWidthMs</t>
   </si>
 </sst>
 </file>
@@ -774,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:A59"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2108,7 @@
         <v>30</v>
       </c>
       <c r="E56" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I56" s="2">
         <v>0</v>
@@ -2186,6 +2201,235 @@
         <v>1</v>
       </c>
       <c r="K59" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B61" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" t="s">
+        <v>116</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="2">
+        <v>1</v>
+      </c>
+      <c r="H61" s="2">
+        <v>20</v>
+      </c>
+      <c r="I61" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="J61" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K61" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" t="s">
+        <v>81</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1</v>
+      </c>
+      <c r="H62" s="2">
+        <v>20</v>
+      </c>
+      <c r="I62" s="2">
+        <v>10</v>
+      </c>
+      <c r="J62" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K62" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B63" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" t="s">
+        <v>84</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G63" s="2">
+        <v>0</v>
+      </c>
+      <c r="H63" s="2">
+        <v>100</v>
+      </c>
+      <c r="I63" s="2">
+        <v>100</v>
+      </c>
+      <c r="J63" s="2">
+        <v>1</v>
+      </c>
+      <c r="K63" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B64" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64" t="s">
+        <v>87</v>
+      </c>
+      <c r="D64" t="s">
+        <v>86</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G64" s="2">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2">
+        <v>50</v>
+      </c>
+      <c r="I64" s="2">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2">
+        <v>1</v>
+      </c>
+      <c r="K64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="C65" t="s">
+        <v>33</v>
+      </c>
+      <c r="D65" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G65" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="H65" s="2">
+        <v>2</v>
+      </c>
+      <c r="I65" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J65" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" t="s">
+        <v>89</v>
+      </c>
+      <c r="D66" t="s">
+        <v>88</v>
+      </c>
+      <c r="E66" s="2">
+        <v>2</v>
+      </c>
+      <c r="I66" s="2">
+        <v>0</v>
+      </c>
+      <c r="K66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B67" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67" t="s">
+        <v>29</v>
+      </c>
+      <c r="D67" t="s">
+        <v>30</v>
+      </c>
+      <c r="E67" s="2">
+        <v>4</v>
+      </c>
+      <c r="I67" s="2">
+        <v>0</v>
+      </c>
+      <c r="K67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B68" t="s">
+        <v>112</v>
+      </c>
+      <c r="C68" t="s">
+        <v>113</v>
+      </c>
+      <c r="D68" t="s">
+        <v>112</v>
+      </c>
+      <c r="E68" s="2">
+        <v>3</v>
+      </c>
+      <c r="I68" s="2">
+        <v>1</v>
+      </c>
+      <c r="K68" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new Chorus effect
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1E391C-7C4A-4F25-84B8-1A00EB08D375}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF27EF7-A72F-4EED-8A5A-60CA0650ECFC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="124">
   <si>
     <t>ratio</t>
   </si>
@@ -391,6 +391,18 @@
   </si>
   <si>
     <t>sweepWidthMs</t>
+  </si>
+  <si>
+    <t>Chorus</t>
+  </si>
+  <si>
+    <t>Number of Voices</t>
+  </si>
+  <si>
+    <t>voiceCount</t>
+  </si>
+  <si>
+    <t>Voice Count</t>
   </si>
 </sst>
 </file>
@@ -789,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,6 +2445,235 @@
         <v>114</v>
       </c>
     </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" t="s">
+        <v>116</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" s="2">
+        <v>10</v>
+      </c>
+      <c r="H70" s="2">
+        <v>50</v>
+      </c>
+      <c r="I70" s="2">
+        <v>30</v>
+      </c>
+      <c r="J70" s="2">
+        <v>1</v>
+      </c>
+      <c r="K70" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" t="s">
+        <v>82</v>
+      </c>
+      <c r="D71" t="s">
+        <v>81</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" s="2">
+        <v>10</v>
+      </c>
+      <c r="H71" s="2">
+        <v>50</v>
+      </c>
+      <c r="I71" s="2">
+        <v>20</v>
+      </c>
+      <c r="J71" s="2">
+        <v>1</v>
+      </c>
+      <c r="K71" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" t="s">
+        <v>85</v>
+      </c>
+      <c r="D72" t="s">
+        <v>84</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G72" s="2">
+        <v>0</v>
+      </c>
+      <c r="H72" s="2">
+        <v>100</v>
+      </c>
+      <c r="I72" s="2">
+        <v>100</v>
+      </c>
+      <c r="J72" s="2">
+        <v>1</v>
+      </c>
+      <c r="K72" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B73" t="s">
+        <v>123</v>
+      </c>
+      <c r="C73" t="s">
+        <v>122</v>
+      </c>
+      <c r="D73" t="s">
+        <v>121</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G73" s="2">
+        <v>0</v>
+      </c>
+      <c r="H73" s="2">
+        <v>50</v>
+      </c>
+      <c r="I73" s="2">
+        <v>2</v>
+      </c>
+      <c r="J73" s="2">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B74" t="s">
+        <v>31</v>
+      </c>
+      <c r="C74" t="s">
+        <v>33</v>
+      </c>
+      <c r="D74" t="s">
+        <v>34</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G74" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="H74" s="2">
+        <v>2</v>
+      </c>
+      <c r="I74" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J74" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K74" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
+        <v>89</v>
+      </c>
+      <c r="D75" t="s">
+        <v>88</v>
+      </c>
+      <c r="E75" s="2">
+        <v>2</v>
+      </c>
+      <c r="I75" s="2">
+        <v>0</v>
+      </c>
+      <c r="K75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" t="s">
+        <v>28</v>
+      </c>
+      <c r="C76" t="s">
+        <v>29</v>
+      </c>
+      <c r="D76" t="s">
+        <v>30</v>
+      </c>
+      <c r="E76" s="2">
+        <v>4</v>
+      </c>
+      <c r="I76" s="2">
+        <v>0</v>
+      </c>
+      <c r="K76" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" t="s">
+        <v>113</v>
+      </c>
+      <c r="D77" t="s">
+        <v>112</v>
+      </c>
+      <c r="E77" s="2">
+        <v>3</v>
+      </c>
+      <c r="I77" s="2">
+        <v>1</v>
+      </c>
+      <c r="K77" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new MVerb (reverb) effect
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF27EF7-A72F-4EED-8A5A-60CA0650ECFC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050E2F84-1FB8-4C52-8CE4-8DD2566C596F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="142">
   <si>
     <t>ratio</t>
   </si>
@@ -403,6 +403,60 @@
   </si>
   <si>
     <t>Voice Count</t>
+  </si>
+  <si>
+    <t>Reverb</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Bandwidth</t>
+  </si>
+  <si>
+    <t>Decay</t>
+  </si>
+  <si>
+    <t>Predelay</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>predelay</t>
+  </si>
+  <si>
+    <t>roomSize</t>
+  </si>
+  <si>
+    <t>dryWetMix</t>
+  </si>
+  <si>
+    <t>damping</t>
+  </si>
+  <si>
+    <t>bandwidth</t>
+  </si>
+  <si>
+    <t>Room Size</t>
+  </si>
+  <si>
+    <t>Damping</t>
+  </si>
+  <si>
+    <t>Late vs Early Mix</t>
+  </si>
+  <si>
+    <t>Early/Late Mix</t>
+  </si>
+  <si>
+    <t>earlyLateMix</t>
   </si>
 </sst>
 </file>
@@ -801,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2674,6 +2728,238 @@
         <v>114</v>
       </c>
     </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" t="s">
+        <v>135</v>
+      </c>
+      <c r="D79" t="s">
+        <v>138</v>
+      </c>
+      <c r="G79" s="2">
+        <v>0</v>
+      </c>
+      <c r="H79" s="2">
+        <v>1</v>
+      </c>
+      <c r="I79" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J79" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K79" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80" t="s">
+        <v>125</v>
+      </c>
+      <c r="C80" t="s">
+        <v>131</v>
+      </c>
+      <c r="D80" t="s">
+        <v>125</v>
+      </c>
+      <c r="G80" s="2">
+        <v>0</v>
+      </c>
+      <c r="H80" s="2">
+        <v>1</v>
+      </c>
+      <c r="I80" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="J80" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K80" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B81" t="s">
+        <v>126</v>
+      </c>
+      <c r="C81" t="s">
+        <v>136</v>
+      </c>
+      <c r="D81" t="s">
+        <v>126</v>
+      </c>
+      <c r="G81" s="2">
+        <v>0</v>
+      </c>
+      <c r="H81" s="2">
+        <v>1</v>
+      </c>
+      <c r="I81" s="2">
+        <v>1</v>
+      </c>
+      <c r="J81" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K81" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B82" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" t="s">
+        <v>69</v>
+      </c>
+      <c r="D82" t="s">
+        <v>127</v>
+      </c>
+      <c r="G82" s="2">
+        <v>0</v>
+      </c>
+      <c r="H82" s="2">
+        <v>1</v>
+      </c>
+      <c r="I82" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="J82" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K82" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B83" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" t="s">
+        <v>132</v>
+      </c>
+      <c r="D83" t="s">
+        <v>128</v>
+      </c>
+      <c r="G83" s="2">
+        <v>0</v>
+      </c>
+      <c r="H83" s="2">
+        <v>1</v>
+      </c>
+      <c r="I83" s="2">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K83" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B84" t="s">
+        <v>129</v>
+      </c>
+      <c r="C84" t="s">
+        <v>133</v>
+      </c>
+      <c r="D84" t="s">
+        <v>137</v>
+      </c>
+      <c r="G84" s="2">
+        <v>0</v>
+      </c>
+      <c r="H84" s="2">
+        <v>1</v>
+      </c>
+      <c r="I84" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J84" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K84" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B85" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" t="s">
+        <v>134</v>
+      </c>
+      <c r="D85" t="s">
+        <v>130</v>
+      </c>
+      <c r="G85" s="2">
+        <v>0</v>
+      </c>
+      <c r="H85" s="2">
+        <v>1</v>
+      </c>
+      <c r="I85" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J85" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K85" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B86" t="s">
+        <v>139</v>
+      </c>
+      <c r="C86" t="s">
+        <v>141</v>
+      </c>
+      <c r="D86" t="s">
+        <v>140</v>
+      </c>
+      <c r="G86" s="2">
+        <v>0</v>
+      </c>
+      <c r="H86" s="2">
+        <v>1</v>
+      </c>
+      <c r="I86" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="J86" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="K86" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new JVerb (JUCE reverb) effect
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050E2F84-1FB8-4C52-8CE4-8DD2566C596F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0300C330-73EF-48DC-85E1-EE06B1F152B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="150">
   <si>
     <t>ratio</t>
   </si>
@@ -405,9 +405,6 @@
     <t>Voice Count</t>
   </si>
   <si>
-    <t>Reverb</t>
-  </si>
-  <si>
     <t>Density</t>
   </si>
   <si>
@@ -457,6 +454,33 @@
   </si>
   <si>
     <t>earlyLateMix</t>
+  </si>
+  <si>
+    <t>Mverb</t>
+  </si>
+  <si>
+    <t>Wet Level</t>
+  </si>
+  <si>
+    <t>Dry Level</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>Freeze Mode</t>
+  </si>
+  <si>
+    <t>freezeMode</t>
+  </si>
+  <si>
+    <t>Freeze</t>
+  </si>
+  <si>
+    <t>JuceVerb</t>
   </si>
 </sst>
 </file>
@@ -855,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:K86"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+      <selection activeCell="A89" sqref="A89:A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,16 +2754,16 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G79" s="2">
         <v>0</v>
@@ -2754,21 +2778,21 @@
         <v>0.01</v>
       </c>
       <c r="K79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B80" t="s">
         <v>124</v>
       </c>
-      <c r="B80" t="s">
-        <v>125</v>
-      </c>
       <c r="C80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G80" s="2">
         <v>0</v>
@@ -2783,21 +2807,21 @@
         <v>0.01</v>
       </c>
       <c r="K80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C81" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G81" s="2">
         <v>0</v>
@@ -2812,21 +2836,21 @@
         <v>0.01</v>
       </c>
       <c r="K81" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B82" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C82" t="s">
         <v>69</v>
       </c>
       <c r="D82" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G82" s="2">
         <v>0</v>
@@ -2846,16 +2870,16 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B83" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D83" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G83" s="2">
         <v>0</v>
@@ -2870,21 +2894,21 @@
         <v>0.01</v>
       </c>
       <c r="K83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B84" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C84" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D84" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G84" s="2">
         <v>0</v>
@@ -2899,21 +2923,21 @@
         <v>0.01</v>
       </c>
       <c r="K84" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D85" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G85" s="2">
         <v>0</v>
@@ -2928,21 +2952,21 @@
         <v>0.01</v>
       </c>
       <c r="K85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="B86" t="s">
+        <v>138</v>
+      </c>
+      <c r="C86" t="s">
+        <v>140</v>
+      </c>
+      <c r="D86" t="s">
         <v>139</v>
-      </c>
-      <c r="C86" t="s">
-        <v>141</v>
-      </c>
-      <c r="D86" t="s">
-        <v>140</v>
       </c>
       <c r="G86" s="2">
         <v>0</v>
@@ -2957,7 +2981,160 @@
         <v>0.01</v>
       </c>
       <c r="K86" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" t="s">
+        <v>132</v>
+      </c>
+      <c r="D88" t="s">
+        <v>136</v>
+      </c>
+      <c r="G88" s="2">
+        <v>0</v>
+      </c>
+      <c r="H88" s="2">
+        <v>1</v>
+      </c>
+      <c r="I88" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K88" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B89" t="s">
+        <v>137</v>
+      </c>
+      <c r="C89" t="s">
+        <v>134</v>
+      </c>
+      <c r="D89" t="s">
+        <v>137</v>
+      </c>
+      <c r="G89" s="2">
+        <v>0</v>
+      </c>
+      <c r="H89" s="2">
+        <v>1</v>
+      </c>
+      <c r="I89" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K89" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B90" t="s">
+        <v>142</v>
+      </c>
+      <c r="C90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" t="s">
+        <v>142</v>
+      </c>
+      <c r="G90" s="2">
+        <v>0</v>
+      </c>
+      <c r="H90" s="2">
+        <v>1</v>
+      </c>
+      <c r="I90" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="K90" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B91" t="s">
+        <v>143</v>
+      </c>
+      <c r="C91" t="s">
+        <v>98</v>
+      </c>
+      <c r="D91" t="s">
+        <v>143</v>
+      </c>
+      <c r="G91" s="2">
+        <v>0</v>
+      </c>
+      <c r="H91" s="2">
+        <v>1</v>
+      </c>
+      <c r="I91" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="K91" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B92" t="s">
+        <v>144</v>
+      </c>
+      <c r="C92" t="s">
+        <v>145</v>
+      </c>
+      <c r="D92" t="s">
+        <v>144</v>
+      </c>
+      <c r="G92" s="2">
+        <v>0</v>
+      </c>
+      <c r="H92" s="2">
+        <v>1</v>
+      </c>
+      <c r="I92" s="2">
+        <v>1</v>
+      </c>
+      <c r="K92" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B93" t="s">
+        <v>146</v>
+      </c>
+      <c r="C93" t="s">
+        <v>147</v>
+      </c>
+      <c r="D93" t="s">
+        <v>148</v>
+      </c>
+      <c r="E93" s="2">
+        <v>2</v>
+      </c>
+      <c r="I93" s="2">
+        <v>0</v>
+      </c>
+      <c r="K93" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Rotary speaker simulation effect
</commit_message>
<xml_diff>
--- a/effects-new/Generator Scripts/Parameters.xlsx
+++ b/effects-new/Generator Scripts/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Github\audio-effects\effects-new\Generator Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0300C330-73EF-48DC-85E1-EE06B1F152B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D3D04D-DE0A-4610-9B72-D78E84446AA4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{793EF1D7-C15C-42F1-9C24-C3733D1F6BC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="153">
   <si>
     <t>ratio</t>
   </si>
@@ -481,6 +481,15 @@
   </si>
   <si>
     <t>JuceVerb</t>
+  </si>
+  <si>
+    <t>Leslie</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>speed</t>
   </si>
 </sst>
 </file>
@@ -879,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3057DDC0-5593-4E02-B6CB-234FA3EDA12D}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89:A93"/>
+      <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3137,6 +3146,35 @@
         <v>147</v>
       </c>
     </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B95" t="s">
+        <v>151</v>
+      </c>
+      <c r="C95" t="s">
+        <v>152</v>
+      </c>
+      <c r="D95" t="s">
+        <v>151</v>
+      </c>
+      <c r="G95" s="2">
+        <v>0</v>
+      </c>
+      <c r="H95" s="2">
+        <v>8</v>
+      </c>
+      <c r="I95" s="2">
+        <v>0</v>
+      </c>
+      <c r="J95" s="2">
+        <v>1</v>
+      </c>
+      <c r="K95" t="s">
+        <v>152</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>